<commit_message>
Final draft of source code
</commit_message>
<xml_diff>
--- a/completeness_reports.xlsx
+++ b/completeness_reports.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
     <t>Fields of Interest</t>
   </si>
@@ -55,16 +55,19 @@
     <t>100.0</t>
   </si>
   <si>
-    <t>98.5</t>
-  </si>
-  <si>
-    <t>97.6</t>
-  </si>
-  <si>
-    <t>98.7</t>
-  </si>
-  <si>
-    <t>99.2</t>
+    <t>99.1</t>
+  </si>
+  <si>
+    <t>97.4</t>
+  </si>
+  <si>
+    <t>97.2</t>
+  </si>
+  <si>
+    <t>96.5</t>
+  </si>
+  <si>
+    <t>91.5</t>
   </si>
   <si>
     <t>ACCESSIONNUMBER</t>
@@ -142,28 +145,22 @@
     <t>FACILITYNAME</t>
   </si>
   <si>
-    <t>99.6</t>
-  </si>
-  <si>
-    <t>99.7</t>
-  </si>
-  <si>
-    <t>99.3</t>
-  </si>
-  <si>
-    <t>31.9</t>
-  </si>
-  <si>
-    <t>11.5</t>
-  </si>
-  <si>
-    <t>32.2</t>
-  </si>
-  <si>
-    <t>60.0</t>
-  </si>
-  <si>
-    <t>34.0</t>
+    <t>93.9</t>
+  </si>
+  <si>
+    <t>31.4</t>
+  </si>
+  <si>
+    <t>24.0</t>
+  </si>
+  <si>
+    <t>19.7</t>
+  </si>
+  <si>
+    <t>16.6</t>
+  </si>
+  <si>
+    <t>22.7</t>
   </si>
 </sst>
 </file>
@@ -549,7 +546,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -563,10 +560,10 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -577,10 +574,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -591,7 +588,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -605,10 +602,10 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -616,13 +613,13 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -633,10 +630,10 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -644,13 +641,13 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -661,10 +658,10 @@
         <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -672,34 +669,34 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="D12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="D13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="D14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
@@ -707,47 +704,47 @@
     </row>
     <row r="15" spans="1:5">
       <c r="D15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="D16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="4:5">
       <c r="D17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="4:5">
       <c r="D18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="4:5">
       <c r="D19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="4:5">
       <c r="D20" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E20" t="s">
         <v>48</v>
@@ -755,7 +752,7 @@
     </row>
     <row r="21" spans="4:5">
       <c r="D21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -763,7 +760,7 @@
     </row>
     <row r="22" spans="4:5">
       <c r="D22" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
@@ -771,15 +768,15 @@
     </row>
     <row r="23" spans="4:5">
       <c r="D23" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="4:5">
       <c r="D24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
         <v>12</v>
@@ -787,15 +784,15 @@
     </row>
     <row r="25" spans="4:5">
       <c r="D25" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="4:5">
       <c r="D26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E26" t="s">
         <v>12</v>

</xml_diff>